<commit_message>
Fix: Edit Services unwanted character.
</commit_message>
<xml_diff>
--- a/imaging_system_app_project/resources/excel/ExcelDatabase.xlsx
+++ b/imaging_system_app_project/resources/excel/ExcelDatabase.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="125">
   <si>
     <t>cust_id</t>
   </si>
@@ -41,7 +41,7 @@
     <t>cust_type</t>
   </si>
   <si>
-    <t>Sample Company 1</t>
+    <t>One Company</t>
   </si>
   <si>
     <t>44734567891</t>
@@ -50,36 +50,45 @@
     <t>One@dummy-mail.com</t>
   </si>
   <si>
-    <t>Sample Company 2</t>
+    <t>Company Two</t>
   </si>
   <si>
     <t>CompanyTwo@dummy-mail.com</t>
   </si>
   <si>
-    <t>Sample Company 3</t>
+    <t>Third Company</t>
   </si>
   <si>
     <t>ThirdC@dummy-mail.com</t>
   </si>
   <si>
-    <t>Sample Company 4</t>
+    <t>4Company</t>
   </si>
   <si>
     <t>4company@dummy-mail.com</t>
   </si>
   <si>
-    <t>Sample Company 5</t>
+    <t>FiveGuys Burger</t>
   </si>
   <si>
     <t>FiveGuys@dummy-mail.com</t>
   </si>
   <si>
-    <t>Sample Company 6</t>
+    <t>6th and Co.</t>
   </si>
   <si>
     <t>6andCo@dummy-mail.com</t>
   </si>
   <si>
+    <t>Dummy</t>
+  </si>
+  <si>
+    <t>44754895625</t>
+  </si>
+  <si>
+    <t>dummy@testcorp.com</t>
+  </si>
+  <si>
     <t>project_id</t>
   </si>
   <si>
@@ -170,6 +179,18 @@
     <t>2021-10-15</t>
   </si>
   <si>
+    <t>2022-02-16</t>
+  </si>
+  <si>
+    <t>This is some test data filling in the specimen procedure information. Please hold till a member of our team is able to speak with you...</t>
+  </si>
+  <si>
+    <t>Test Data....</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>service_id</t>
   </si>
   <si>
@@ -239,6 +260,12 @@
     <t>Cryopreparation: LR white</t>
   </si>
   <si>
+    <t>Test Service</t>
+  </si>
+  <si>
+    <t>Boris</t>
+  </si>
+  <si>
     <t>worker_id</t>
   </si>
   <si>
@@ -287,6 +314,15 @@
     <t>John-CompanyTwo@dummy-mail.com</t>
   </si>
   <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>44765496216</t>
+  </si>
+  <si>
+    <t>john@doe.com</t>
+  </si>
+  <si>
     <t>worker_project_bridge_id</t>
   </si>
   <si>
@@ -341,10 +377,7 @@
     <t>2021-11-12</t>
   </si>
   <si>
-    <t>120 University Place, Glasgow G12 8TA</t>
-  </si>
-  <si>
-    <t>Extra - Annual charge</t>
+    <t>143, Fake street, Glasg</t>
   </si>
   <si>
     <t>2021-11-22</t>
@@ -353,10 +386,16 @@
     <t>111, DumDum street, Dum City</t>
   </si>
   <si>
-    <t>Sample extra 1</t>
-  </si>
-  <si>
-    <t>Sample extra 2</t>
+    <t>2022-02-15</t>
+  </si>
+  <si>
+    <t>Address, GL12 3BC</t>
+  </si>
+  <si>
+    <t>First Service</t>
+  </si>
+  <si>
+    <t>Second Service</t>
   </si>
 </sst>
 </file>
@@ -688,7 +727,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -834,6 +873,26 @@
         <v>1.5</v>
       </c>
     </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8">
+        <v>119</v>
+      </c>
+      <c r="F8">
+        <v>1.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -841,7 +900,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X7"/>
+  <dimension ref="A1:X8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -849,76 +908,76 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="K1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="L1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="M1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="N1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="O1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="P1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="Q1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="R1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="S1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="T1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="U1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="V1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="W1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="X1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:24">
@@ -926,16 +985,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="V2">
         <v>0</v>
       </c>
       <c r="W2">
-        <v>260</v>
+        <v>50</v>
       </c>
       <c r="X2">
         <v>1</v>
@@ -946,7 +1005,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -966,7 +1025,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C4">
         <v>18</v>
@@ -986,7 +1045,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C5">
         <v>9</v>
@@ -1006,7 +1065,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C6">
         <v>7</v>
@@ -1026,7 +1085,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C7">
         <v>11</v>
@@ -1039,6 +1098,80 @@
       </c>
       <c r="X7">
         <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" t="s">
+        <v>54</v>
+      </c>
+      <c r="M8" t="s">
+        <v>54</v>
+      </c>
+      <c r="N8" t="s">
+        <v>54</v>
+      </c>
+      <c r="O8" t="s">
+        <v>54</v>
+      </c>
+      <c r="P8" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>54</v>
+      </c>
+      <c r="R8" t="s">
+        <v>54</v>
+      </c>
+      <c r="S8" t="s">
+        <v>54</v>
+      </c>
+      <c r="T8" t="s">
+        <v>54</v>
+      </c>
+      <c r="U8" t="s">
+        <v>54</v>
+      </c>
+      <c r="V8">
+        <v>2</v>
+      </c>
+      <c r="W8">
+        <v>4050</v>
+      </c>
+      <c r="X8">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1048,7 +1181,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1056,22 +1189,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1079,7 +1212,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -1091,7 +1224,7 @@
         <v>75</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1099,7 +1232,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C3">
         <v>55</v>
@@ -1111,7 +1244,7 @@
         <v>82.5</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1119,7 +1252,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -1131,7 +1264,7 @@
         <v>150</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1139,7 +1272,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C5">
         <v>40</v>
@@ -1151,7 +1284,7 @@
         <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1159,7 +1292,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C6">
         <v>50</v>
@@ -1171,7 +1304,7 @@
         <v>75</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1179,7 +1312,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -1191,7 +1324,7 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1199,7 +1332,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C8">
         <v>100</v>
@@ -1211,7 +1344,7 @@
         <v>150</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1219,7 +1352,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C9">
         <v>200</v>
@@ -1231,7 +1364,7 @@
         <v>300</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1239,7 +1372,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C10">
         <v>40</v>
@@ -1251,7 +1384,7 @@
         <v>60</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1259,7 +1392,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C11">
         <v>70</v>
@@ -1271,7 +1404,7 @@
         <v>105</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1279,7 +1412,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="C12">
         <v>150</v>
@@ -1291,7 +1424,7 @@
         <v>225</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1299,7 +1432,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C13">
         <v>100</v>
@@ -1311,7 +1444,7 @@
         <v>150</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1319,7 +1452,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C14">
         <v>80</v>
@@ -1331,7 +1464,47 @@
         <v>120</v>
       </c>
       <c r="F14" t="s">
-        <v>59</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15">
+        <v>50</v>
+      </c>
+      <c r="D15">
+        <v>25</v>
+      </c>
+      <c r="E15">
+        <v>75</v>
+      </c>
+      <c r="F15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16">
+        <v>300</v>
+      </c>
+      <c r="D16">
+        <v>150</v>
+      </c>
+      <c r="E16">
+        <v>450</v>
+      </c>
+      <c r="F16" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1341,7 +1514,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1349,19 +1522,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1369,13 +1542,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1386,13 +1559,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1403,13 +1576,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1420,13 +1593,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1437,13 +1610,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1454,16 +1627,33 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="E7">
         <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1481,13 +1671,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1547,24 +1737,24 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1574,7 +1764,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1582,19 +1772,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="D1" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="E1" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1704,16 +1894,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1721,16 +1911,84 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C9">
+        <v>200</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>200</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
         <v>10</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>160</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
         <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>4050</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1740,7 +1998,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1748,13 +2006,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1821,6 +2079,28 @@
       </c>
       <c r="C7">
         <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1830,7 +2110,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1838,31 +2118,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="E1" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="F1" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="G1" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="H1" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1870,19 +2150,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="H2">
-        <v>490</v>
+        <v>180</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1893,28 +2167,62 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E3">
+        <v>120</v>
+      </c>
+      <c r="H3">
+        <v>292.5</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H4">
+        <v>82.5</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
-        <v>111</v>
-      </c>
-      <c r="G3">
-        <v>20</v>
-      </c>
-      <c r="H3">
-        <v>322.5</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
+      <c r="F5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G5">
+        <v>25</v>
+      </c>
+      <c r="H5">
+        <v>4085</v>
+      </c>
+      <c r="I5">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: update the correct static files
</commit_message>
<xml_diff>
--- a/imaging_system_app_project/resources/excel/ExcelDatabase.xlsx
+++ b/imaging_system_app_project/resources/excel/ExcelDatabase.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="112">
   <si>
     <t>cust_id</t>
   </si>
@@ -41,7 +41,7 @@
     <t>cust_type</t>
   </si>
   <si>
-    <t>One Company</t>
+    <t>Sample Company 1</t>
   </si>
   <si>
     <t>44734567891</t>
@@ -50,45 +50,36 @@
     <t>One@dummy-mail.com</t>
   </si>
   <si>
-    <t>Company Two</t>
+    <t>Sample Company 2</t>
   </si>
   <si>
     <t>CompanyTwo@dummy-mail.com</t>
   </si>
   <si>
-    <t>Third Company</t>
+    <t>Sample Company 3</t>
   </si>
   <si>
     <t>ThirdC@dummy-mail.com</t>
   </si>
   <si>
-    <t>4Company</t>
+    <t>Sample Company 4</t>
   </si>
   <si>
     <t>4company@dummy-mail.com</t>
   </si>
   <si>
-    <t>FiveGuys Burger</t>
+    <t>Sample Company 5</t>
   </si>
   <si>
     <t>FiveGuys@dummy-mail.com</t>
   </si>
   <si>
-    <t>6th and Co.</t>
+    <t>Sample Company 6</t>
   </si>
   <si>
     <t>6andCo@dummy-mail.com</t>
   </si>
   <si>
-    <t>Dummy</t>
-  </si>
-  <si>
-    <t>44754895625</t>
-  </si>
-  <si>
-    <t>dummy@testcorp.com</t>
-  </si>
-  <si>
     <t>project_id</t>
   </si>
   <si>
@@ -179,18 +170,6 @@
     <t>2021-10-15</t>
   </si>
   <si>
-    <t>2022-02-16</t>
-  </si>
-  <si>
-    <t>This is some test data filling in the specimen procedure information. Please hold till a member of our team is able to speak with you...</t>
-  </si>
-  <si>
-    <t>Test Data....</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>service_id</t>
   </si>
   <si>
@@ -260,12 +239,6 @@
     <t>Cryopreparation: LR white</t>
   </si>
   <si>
-    <t>Test Service</t>
-  </si>
-  <si>
-    <t>Boris</t>
-  </si>
-  <si>
     <t>worker_id</t>
   </si>
   <si>
@@ -314,15 +287,6 @@
     <t>John-CompanyTwo@dummy-mail.com</t>
   </si>
   <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>44765496216</t>
-  </si>
-  <si>
-    <t>john@doe.com</t>
-  </si>
-  <si>
     <t>worker_project_bridge_id</t>
   </si>
   <si>
@@ -377,7 +341,10 @@
     <t>2021-11-12</t>
   </si>
   <si>
-    <t>143, Fake street, Glasg</t>
+    <t>120 University Place, Glasgow G12 8TA</t>
+  </si>
+  <si>
+    <t>Extra - Annual charge</t>
   </si>
   <si>
     <t>2021-11-22</t>
@@ -386,16 +353,10 @@
     <t>111, DumDum street, Dum City</t>
   </si>
   <si>
-    <t>2022-02-15</t>
-  </si>
-  <si>
-    <t>Address, GL12 3BC</t>
-  </si>
-  <si>
-    <t>First Service</t>
-  </si>
-  <si>
-    <t>Second Service</t>
+    <t>Sample extra 1</t>
+  </si>
+  <si>
+    <t>Sample extra 2</t>
   </si>
 </sst>
 </file>
@@ -727,7 +688,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -873,26 +834,6 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8">
-        <v>119</v>
-      </c>
-      <c r="F8">
-        <v>1.5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -900,7 +841,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X8"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -908,76 +849,76 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>30</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>31</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>32</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>33</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>34</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>35</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>36</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>38</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>39</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>40</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>41</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>42</v>
-      </c>
-      <c r="V1" t="s">
-        <v>43</v>
-      </c>
-      <c r="W1" t="s">
-        <v>44</v>
-      </c>
-      <c r="X1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:24">
@@ -985,16 +926,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="V2">
         <v>0</v>
       </c>
       <c r="W2">
-        <v>50</v>
+        <v>260</v>
       </c>
       <c r="X2">
         <v>1</v>
@@ -1005,7 +946,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -1025,7 +966,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4">
         <v>18</v>
@@ -1045,7 +986,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C5">
         <v>9</v>
@@ -1065,7 +1006,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C6">
         <v>7</v>
@@ -1085,7 +1026,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C7">
         <v>11</v>
@@ -1098,80 +1039,6 @@
       </c>
       <c r="X7">
         <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" t="s">
-        <v>54</v>
-      </c>
-      <c r="J8" t="s">
-        <v>54</v>
-      </c>
-      <c r="K8" t="s">
-        <v>55</v>
-      </c>
-      <c r="L8" t="s">
-        <v>54</v>
-      </c>
-      <c r="M8" t="s">
-        <v>54</v>
-      </c>
-      <c r="N8" t="s">
-        <v>54</v>
-      </c>
-      <c r="O8" t="s">
-        <v>54</v>
-      </c>
-      <c r="P8" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>54</v>
-      </c>
-      <c r="R8" t="s">
-        <v>54</v>
-      </c>
-      <c r="S8" t="s">
-        <v>54</v>
-      </c>
-      <c r="T8" t="s">
-        <v>54</v>
-      </c>
-      <c r="U8" t="s">
-        <v>54</v>
-      </c>
-      <c r="V8">
-        <v>2</v>
-      </c>
-      <c r="W8">
-        <v>4050</v>
-      </c>
-      <c r="X8">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1181,7 +1048,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1189,22 +1056,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1212,7 +1079,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -1224,7 +1091,7 @@
         <v>75</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1232,7 +1099,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C3">
         <v>55</v>
@@ -1244,7 +1111,7 @@
         <v>82.5</v>
       </c>
       <c r="F3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1252,7 +1119,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -1264,7 +1131,7 @@
         <v>150</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1272,7 +1139,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C5">
         <v>40</v>
@@ -1284,7 +1151,7 @@
         <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1292,7 +1159,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C6">
         <v>50</v>
@@ -1304,7 +1171,7 @@
         <v>75</v>
       </c>
       <c r="F6" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1312,7 +1179,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -1324,7 +1191,7 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1332,7 +1199,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C8">
         <v>100</v>
@@ -1344,7 +1211,7 @@
         <v>150</v>
       </c>
       <c r="F8" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1352,7 +1219,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C9">
         <v>200</v>
@@ -1364,7 +1231,7 @@
         <v>300</v>
       </c>
       <c r="F9" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1372,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C10">
         <v>40</v>
@@ -1384,7 +1251,7 @@
         <v>60</v>
       </c>
       <c r="F10" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1392,7 +1259,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C11">
         <v>70</v>
@@ -1404,7 +1271,7 @@
         <v>105</v>
       </c>
       <c r="F11" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1412,7 +1279,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C12">
         <v>150</v>
@@ -1424,7 +1291,7 @@
         <v>225</v>
       </c>
       <c r="F12" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1432,7 +1299,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C13">
         <v>100</v>
@@ -1444,7 +1311,7 @@
         <v>150</v>
       </c>
       <c r="F13" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1452,7 +1319,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C14">
         <v>80</v>
@@ -1464,47 +1331,7 @@
         <v>120</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15">
-        <v>50</v>
-      </c>
-      <c r="D15">
-        <v>25</v>
-      </c>
-      <c r="E15">
-        <v>75</v>
-      </c>
-      <c r="F15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16">
-        <v>300</v>
-      </c>
-      <c r="D16">
-        <v>150</v>
-      </c>
-      <c r="E16">
-        <v>450</v>
-      </c>
-      <c r="F16" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1514,7 +1341,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1522,19 +1349,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1542,13 +1369,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1559,13 +1386,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1576,13 +1403,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1593,13 +1420,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1610,13 +1437,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1627,33 +1454,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E7">
         <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" t="s">
-        <v>98</v>
-      </c>
-      <c r="D8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E8">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1671,13 +1481,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C1" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1737,24 +1547,24 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1764,7 +1574,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1772,19 +1582,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C1" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="D1" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="E1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1894,16 +1704,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1911,84 +1721,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>200</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>160</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <v>50</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
         <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>9</v>
-      </c>
-      <c r="C13">
-        <v>4050</v>
-      </c>
-      <c r="D13">
-        <v>7</v>
-      </c>
-      <c r="E13">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1998,7 +1740,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2006,13 +1748,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2079,28 +1821,6 @@
       </c>
       <c r="C7">
         <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2110,7 +1830,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2118,31 +1838,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="E1" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="F1" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="G1" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="H1" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="I1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2150,13 +1870,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>106</v>
+      </c>
+      <c r="D2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
       </c>
       <c r="H2">
-        <v>180</v>
+        <v>490</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -2167,62 +1893,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>109</v>
+      </c>
+      <c r="D3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
       </c>
       <c r="H3">
-        <v>292.5</v>
+        <v>322.5</v>
       </c>
       <c r="I3">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C4" t="s">
-        <v>122</v>
-      </c>
-      <c r="H4">
-        <v>82.5</v>
-      </c>
-      <c r="I4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G5">
-        <v>25</v>
-      </c>
-      <c r="H5">
-        <v>4085</v>
-      </c>
-      <c r="I5">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fix - headers appearing when all projects,services,customers and bills lists are empty
</commit_message>
<xml_diff>
--- a/imaging_system_app_project/resources/excel/ExcelDatabase.xlsx
+++ b/imaging_system_app_project/resources/excel/ExcelDatabase.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="113">
   <si>
     <t>cust_id</t>
   </si>
@@ -41,40 +41,43 @@
     <t>cust_type</t>
   </si>
   <si>
-    <t>Sample Company 1</t>
+    <t>One Company</t>
+  </si>
+  <si>
+    <t>44734567890</t>
+  </si>
+  <si>
+    <t>One@dummy-mail.com</t>
+  </si>
+  <si>
+    <t>Company Two</t>
   </si>
   <si>
     <t>44734567891</t>
   </si>
   <si>
-    <t>One@dummy-mail.com</t>
-  </si>
-  <si>
-    <t>Sample Company 2</t>
-  </si>
-  <si>
     <t>CompanyTwo@dummy-mail.com</t>
   </si>
   <si>
-    <t>Sample Company 3</t>
+    <t>Third Company</t>
   </si>
   <si>
     <t>ThirdC@dummy-mail.com</t>
   </si>
   <si>
-    <t>Sample Company 4</t>
+    <t>4Company</t>
   </si>
   <si>
     <t>4company@dummy-mail.com</t>
   </si>
   <si>
-    <t>Sample Company 5</t>
+    <t>FiveGuys Burger</t>
   </si>
   <si>
     <t>FiveGuys@dummy-mail.com</t>
   </si>
   <si>
-    <t>Sample Company 6</t>
+    <t>6th and Co.</t>
   </si>
   <si>
     <t>6andCo@dummy-mail.com</t>
@@ -239,6 +242,12 @@
     <t>Cryopreparation: LR white</t>
   </si>
   <si>
+    <t>JEOL 6000</t>
+  </si>
+  <si>
+    <t>JEOL 10000</t>
+  </si>
+  <si>
     <t>worker_id</t>
   </si>
   <si>
@@ -351,12 +360,6 @@
   </si>
   <si>
     <t>111, DumDum street, Dum City</t>
-  </si>
-  <si>
-    <t>Sample extra 1</t>
-  </si>
-  <si>
-    <t>Sample extra 2</t>
   </si>
 </sst>
 </file>
@@ -742,10 +745,10 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>103</v>
@@ -759,13 +762,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4">
         <v>112</v>
@@ -779,13 +782,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>105</v>
@@ -799,13 +802,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6">
         <v>121</v>
@@ -819,13 +822,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E7">
         <v>116</v>
@@ -849,76 +852,76 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="W1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:24">
@@ -926,16 +929,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W2">
-        <v>260</v>
+        <v>290</v>
       </c>
       <c r="X2">
         <v>1</v>
@@ -946,7 +949,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -966,7 +969,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C4">
         <v>18</v>
@@ -975,7 +978,7 @@
         <v>2</v>
       </c>
       <c r="W4">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="X4">
         <v>1</v>
@@ -986,7 +989,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C5">
         <v>9</v>
@@ -1006,7 +1009,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <v>7</v>
@@ -1026,7 +1029,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C7">
         <v>11</v>
@@ -1048,7 +1051,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1056,22 +1059,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1079,19 +1082,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D2">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E2">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1099,7 +1102,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C3">
         <v>55</v>
@@ -1111,7 +1114,7 @@
         <v>82.5</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1119,7 +1122,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -1131,7 +1134,7 @@
         <v>150</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1139,7 +1142,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C5">
         <v>40</v>
@@ -1151,7 +1154,7 @@
         <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1159,7 +1162,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C6">
         <v>50</v>
@@ -1171,7 +1174,7 @@
         <v>75</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1179,7 +1182,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -1191,7 +1194,7 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1199,7 +1202,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C8">
         <v>100</v>
@@ -1211,7 +1214,7 @@
         <v>150</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1219,7 +1222,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C9">
         <v>200</v>
@@ -1231,7 +1234,7 @@
         <v>300</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1239,7 +1242,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C10">
         <v>40</v>
@@ -1251,7 +1254,7 @@
         <v>60</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1259,7 +1262,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C11">
         <v>70</v>
@@ -1271,7 +1274,7 @@
         <v>105</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1279,7 +1282,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C12">
         <v>150</v>
@@ -1291,7 +1294,7 @@
         <v>225</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1299,7 +1302,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C13">
         <v>100</v>
@@ -1311,7 +1314,7 @@
         <v>150</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1319,7 +1322,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C14">
         <v>80</v>
@@ -1331,7 +1334,47 @@
         <v>120</v>
       </c>
       <c r="F14" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15">
+        <v>70</v>
+      </c>
+      <c r="D15">
+        <v>35</v>
+      </c>
+      <c r="E15">
+        <v>105</v>
+      </c>
+      <c r="F15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16">
+        <v>100</v>
+      </c>
+      <c r="D16">
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <v>150</v>
+      </c>
+      <c r="F16" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1349,19 +1392,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1369,13 +1412,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1386,13 +1429,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1403,13 +1446,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1420,13 +1463,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1437,13 +1480,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1454,13 +1497,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1481,13 +1524,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1547,24 +1590,24 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1582,19 +1625,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
         <v>92</v>
       </c>
-      <c r="C1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" t="s">
-        <v>89</v>
-      </c>
       <c r="E1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1605,7 +1648,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1639,7 +1682,7 @@
         <v>1.5</v>
       </c>
       <c r="C4">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1748,13 +1791,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1838,31 +1881,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="G1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1870,19 +1913,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="H2">
-        <v>490</v>
+        <v>585</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1893,25 +1936,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>111</v>
-      </c>
-      <c r="G3">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="H3">
-        <v>322.5</v>
+        <v>292.5</v>
       </c>
       <c r="I3">
         <v>2</v>

</xml_diff>

<commit_message>
feat: adds a project list to view bill
</commit_message>
<xml_diff>
--- a/imaging_system_app_project/resources/excel/ExcelDatabase.xlsx
+++ b/imaging_system_app_project/resources/excel/ExcelDatabase.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="109">
   <si>
     <t>cust_id</t>
   </si>
@@ -44,7 +44,7 @@
     <t>One Company</t>
   </si>
   <si>
-    <t>44734567890</t>
+    <t>44734567891</t>
   </si>
   <si>
     <t>One@dummy-mail.com</t>
@@ -53,9 +53,6 @@
     <t>Company Two</t>
   </si>
   <si>
-    <t>44734567891</t>
-  </si>
-  <si>
     <t>CompanyTwo@dummy-mail.com</t>
   </si>
   <si>
@@ -182,10 +179,7 @@
     <t>normal_price</t>
   </si>
   <si>
-    <t>in_house_price</t>
-  </si>
-  <si>
-    <t>outside_price</t>
+    <t>external_price</t>
   </si>
   <si>
     <t>unit_name</t>
@@ -240,12 +234,6 @@
   </si>
   <si>
     <t>Cryopreparation: LR white</t>
-  </si>
-  <si>
-    <t>JEOL 6000</t>
-  </si>
-  <si>
-    <t>JEOL 10000</t>
   </si>
   <si>
     <t>worker_id</t>
@@ -745,10 +733,10 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
       </c>
       <c r="E3">
         <v>103</v>
@@ -762,13 +750,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
       </c>
       <c r="E4">
         <v>112</v>
@@ -782,13 +770,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
       </c>
       <c r="E5">
         <v>105</v>
@@ -802,13 +790,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
       </c>
       <c r="E6">
         <v>121</v>
@@ -822,13 +810,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
       </c>
       <c r="E7">
         <v>116</v>
@@ -852,76 +840,76 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>31</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>32</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>33</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>34</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>36</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>37</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>38</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>39</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>40</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>41</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>42</v>
-      </c>
-      <c r="X1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:24">
@@ -929,16 +917,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>290</v>
+        <v>260</v>
       </c>
       <c r="X2">
         <v>1</v>
@@ -949,7 +937,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -969,7 +957,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4">
         <v>18</v>
@@ -978,7 +966,7 @@
         <v>2</v>
       </c>
       <c r="W4">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="X4">
         <v>1</v>
@@ -989,7 +977,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5">
         <v>9</v>
@@ -1009,7 +997,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6">
         <v>7</v>
@@ -1029,7 +1017,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7">
         <v>11</v>
@@ -1051,330 +1039,248 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>53</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>54</v>
       </c>
-      <c r="F1" t="s">
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>56</v>
-      </c>
-      <c r="C2">
-        <v>80</v>
-      </c>
-      <c r="D2">
-        <v>40</v>
-      </c>
-      <c r="E2">
-        <v>120</v>
-      </c>
-      <c r="F2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>58</v>
       </c>
       <c r="C3">
         <v>55</v>
       </c>
       <c r="D3">
-        <v>27.5</v>
-      </c>
-      <c r="E3">
         <v>82.5</v>
       </c>
-      <c r="F3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C4">
         <v>100</v>
       </c>
       <c r="D4">
-        <v>50</v>
-      </c>
-      <c r="E4">
         <v>150</v>
       </c>
-      <c r="F4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C5">
         <v>40</v>
       </c>
       <c r="D5">
-        <v>20</v>
-      </c>
-      <c r="E5">
         <v>60</v>
       </c>
-      <c r="F5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C6">
         <v>50</v>
       </c>
       <c r="D6">
-        <v>25</v>
-      </c>
-      <c r="E6">
         <v>75</v>
       </c>
-      <c r="F6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7">
         <v>10</v>
       </c>
       <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="E7">
         <v>15</v>
       </c>
-      <c r="F7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="E7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C8">
         <v>100</v>
       </c>
       <c r="D8">
-        <v>50</v>
-      </c>
-      <c r="E8">
         <v>150</v>
       </c>
-      <c r="F8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="E8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C9">
         <v>200</v>
       </c>
       <c r="D9">
-        <v>100</v>
-      </c>
-      <c r="E9">
         <v>300</v>
       </c>
-      <c r="F9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C10">
         <v>40</v>
       </c>
       <c r="D10">
-        <v>20</v>
-      </c>
-      <c r="E10">
         <v>60</v>
       </c>
-      <c r="F10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="E10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C11">
         <v>70</v>
       </c>
       <c r="D11">
-        <v>35</v>
-      </c>
-      <c r="E11">
         <v>105</v>
       </c>
-      <c r="F11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="E11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C12">
         <v>150</v>
       </c>
       <c r="D12">
-        <v>75</v>
-      </c>
-      <c r="E12">
         <v>225</v>
       </c>
-      <c r="F12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="E12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C13">
         <v>100</v>
       </c>
       <c r="D13">
-        <v>50</v>
-      </c>
-      <c r="E13">
         <v>150</v>
       </c>
-      <c r="F13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14">
         <v>80</v>
       </c>
       <c r="D14">
-        <v>40</v>
-      </c>
-      <c r="E14">
         <v>120</v>
       </c>
-      <c r="F14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15">
-        <v>70</v>
-      </c>
-      <c r="D15">
-        <v>35</v>
-      </c>
-      <c r="E15">
-        <v>105</v>
-      </c>
-      <c r="F15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16">
-        <v>100</v>
-      </c>
-      <c r="D16">
-        <v>50</v>
-      </c>
-      <c r="E16">
-        <v>150</v>
-      </c>
-      <c r="F16" t="s">
-        <v>57</v>
+      <c r="E14" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1392,19 +1298,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1412,13 +1318,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1429,13 +1335,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1446,13 +1352,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1463,13 +1369,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1480,13 +1386,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1497,13 +1403,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1524,13 +1430,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1625,19 +1531,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1648,7 +1554,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1682,7 +1588,7 @@
         <v>1.5</v>
       </c>
       <c r="C4">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1791,13 +1697,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1881,31 +1787,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" t="s">
         <v>100</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>101</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>102</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>103</v>
       </c>
-      <c r="E1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H1" t="s">
-        <v>107</v>
-      </c>
       <c r="I1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1913,19 +1819,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E2">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="H2">
-        <v>585</v>
+        <v>490</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1936,10 +1842,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H3">
         <v>292.5</v>

</xml_diff>